<commit_message>
teleporter implemented + updated visuals
</commit_message>
<xml_diff>
--- a/Data/LevelLayout0.xlsx
+++ b/Data/LevelLayout0.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\saril\Documents\GitHub\Programming4\2DAE14_Janssen_Sari_Tron\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2B13273-6732-4D3A-89B8-7826685EADAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED013ACE-6C39-4CD8-B60D-EC3D15E8FD16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-8550" yWindow="1935" windowWidth="17280" windowHeight="8970" xr2:uid="{4DA9D7AD-EAE2-43E4-A737-467F9E8D8689}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4DA9D7AD-EAE2-43E4-A737-467F9E8D8689}"/>
   </bookViews>
   <sheets>
     <sheet name="LevelLayout0" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -88,6 +88,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF7030A0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -116,7 +122,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -124,6 +130,7 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -441,7 +448,7 @@
   <dimension ref="A1:BF54"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AD22" sqref="AD22"/>
+      <selection activeCell="AC27" sqref="AC27:AD28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5088,34 +5095,34 @@
         <v>1</v>
       </c>
       <c r="U27" s="6">
+        <v>6</v>
+      </c>
+      <c r="V27" s="6">
+        <v>6</v>
+      </c>
+      <c r="W27" s="3">
+        <v>1</v>
+      </c>
+      <c r="X27" s="1">
+        <v>0</v>
+      </c>
+      <c r="Y27" s="1">
+        <v>0</v>
+      </c>
+      <c r="Z27" s="1">
+        <v>0</v>
+      </c>
+      <c r="AA27" s="1">
+        <v>0</v>
+      </c>
+      <c r="AB27" s="3">
+        <v>1</v>
+      </c>
+      <c r="AC27" s="7">
         <v>3</v>
       </c>
-      <c r="V27" s="6">
+      <c r="AD27" s="7">
         <v>3</v>
-      </c>
-      <c r="W27" s="3">
-        <v>1</v>
-      </c>
-      <c r="X27" s="1">
-        <v>0</v>
-      </c>
-      <c r="Y27" s="1">
-        <v>0</v>
-      </c>
-      <c r="Z27" s="1">
-        <v>0</v>
-      </c>
-      <c r="AA27" s="1">
-        <v>0</v>
-      </c>
-      <c r="AB27" s="3">
-        <v>1</v>
-      </c>
-      <c r="AC27" s="3">
-        <v>1</v>
-      </c>
-      <c r="AD27" s="3">
-        <v>1</v>
       </c>
       <c r="AE27" s="3">
         <v>1</v>
@@ -5264,34 +5271,34 @@
         <v>1</v>
       </c>
       <c r="U28" s="6">
+        <v>6</v>
+      </c>
+      <c r="V28" s="6">
+        <v>6</v>
+      </c>
+      <c r="W28" s="3">
+        <v>1</v>
+      </c>
+      <c r="X28" s="1">
+        <v>0</v>
+      </c>
+      <c r="Y28" s="1">
+        <v>0</v>
+      </c>
+      <c r="Z28" s="1">
+        <v>0</v>
+      </c>
+      <c r="AA28" s="1">
+        <v>0</v>
+      </c>
+      <c r="AB28" s="3">
+        <v>1</v>
+      </c>
+      <c r="AC28" s="7">
         <v>3</v>
       </c>
-      <c r="V28" s="6">
+      <c r="AD28" s="7">
         <v>3</v>
-      </c>
-      <c r="W28" s="3">
-        <v>1</v>
-      </c>
-      <c r="X28" s="1">
-        <v>0</v>
-      </c>
-      <c r="Y28" s="1">
-        <v>0</v>
-      </c>
-      <c r="Z28" s="1">
-        <v>0</v>
-      </c>
-      <c r="AA28" s="1">
-        <v>0</v>
-      </c>
-      <c r="AB28" s="3">
-        <v>1</v>
-      </c>
-      <c r="AC28" s="3">
-        <v>1</v>
-      </c>
-      <c r="AD28" s="3">
-        <v>1</v>
       </c>
       <c r="AE28" s="3">
         <v>1</v>
@@ -7636,10 +7643,10 @@
         <v>1</v>
       </c>
       <c r="AW41" s="6">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="AX41" s="6">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="AY41" s="3">
         <v>1</v>
@@ -7812,10 +7819,10 @@
         <v>1</v>
       </c>
       <c r="AW42" s="6">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="AX42" s="6">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="AY42" s="3">
         <v>1</v>

</xml_diff>